<commit_message>
Rider Link Modal Created
</commit_message>
<xml_diff>
--- a/เอกสารPnP/PnP_Info_Request.xlsx
+++ b/เอกสารPnP/PnP_Info_Request.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pree_site\Puff n Pie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pree_site\Puff n Pie\เอกสารPnP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3795" windowHeight="2760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ขอมูลทั่วไป" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="103">
   <si>
     <t>เมนูแนะนำ/ใหม่</t>
   </si>
@@ -318,6 +318,27 @@
   </si>
   <si>
     <t>https://www.facebook.com/PuffandPieOfficial</t>
+  </si>
+  <si>
+    <t>ส่งไฟล์ภาพ</t>
+  </si>
+  <si>
+    <t>รายละเอียดไฟล์ภาพ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3 ภาพต่อหนึ่งกิจกรรม </t>
+  </si>
+  <si>
+    <t>ขนาดดังนี้ (กxย) px</t>
+  </si>
+  <si>
+    <t xml:space="preserve">900 x 600  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">900 x 500 </t>
+  </si>
+  <si>
+    <t>450 x 450</t>
   </si>
 </sst>
 </file>
@@ -325,8 +346,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000000000"/>
-    <numFmt numFmtId="169" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -361,12 +382,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="22">
@@ -625,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -661,70 +688,83 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1008,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,32 +1064,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1093,13 +1133,13 @@
       <c r="C4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="20">
         <v>44393</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="20">
         <v>44407</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="20" t="s">
         <v>35</v>
       </c>
       <c r="G4" s="5" t="s">
@@ -1111,7 +1151,7 @@
       <c r="I4" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="34" t="s">
+      <c r="J4" s="27" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1165,18 +1205,18 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1210,10 +1250,10 @@
       <c r="C12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="26" t="s">
         <v>91</v>
       </c>
       <c r="F12" s="12"/>
@@ -1251,17 +1291,17 @@
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="30"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1282,7 +1322,7 @@
       <c r="B20" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="27" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1311,7 +1351,7 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H30" s="31"/>
+      <c r="H30" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1350,32 +1390,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="17"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1402,7 +1442,7 @@
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="3" t="s">
@@ -1410,7 +1450,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1431,10 +1471,10 @@
       <c r="G4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="7" t="s">
@@ -1442,7 +1482,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1454,7 +1494,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1466,7 +1506,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1478,7 +1518,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -1491,18 +1531,18 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="17"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1529,7 +1569,7 @@
       <c r="H11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J11" s="3" t="s">
@@ -1537,7 +1577,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1558,10 +1598,10 @@
       <c r="G12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J12" s="7" t="s">
@@ -1569,7 +1609,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1581,7 +1621,7 @@
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1593,7 +1633,7 @@
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1605,7 +1645,7 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -1618,18 +1658,18 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="17"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1656,7 +1696,7 @@
       <c r="H19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="I19" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J19" s="3" t="s">
@@ -1664,7 +1704,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1685,10 +1725,10 @@
       <c r="G20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="I20" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J20" s="7" t="s">
@@ -1696,7 +1736,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1708,7 +1748,7 @@
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1720,7 +1760,7 @@
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1732,7 +1772,7 @@
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -1745,18 +1785,18 @@
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="17"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="14"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1783,7 +1823,7 @@
       <c r="H27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I27" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J27" s="3" t="s">
@@ -1791,7 +1831,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1812,10 +1852,10 @@
       <c r="G28" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J28" s="7" t="s">
@@ -1823,7 +1863,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -1835,7 +1875,7 @@
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1847,7 +1887,7 @@
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -1859,7 +1899,7 @@
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -1872,18 +1912,18 @@
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="17"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="14"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -1910,7 +1950,7 @@
       <c r="H35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I35" s="18" t="s">
+      <c r="I35" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J35" s="3" t="s">
@@ -1918,7 +1958,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1939,10 +1979,10 @@
       <c r="G36" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H36" s="22" t="s">
+      <c r="H36" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I36" s="22" t="s">
+      <c r="I36" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J36" s="7" t="s">
@@ -1950,7 +1990,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -1962,7 +2002,7 @@
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -1974,7 +2014,7 @@
       <c r="J38" s="7"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
+      <c r="A39" s="17"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -1986,7 +2026,7 @@
       <c r="J39" s="7"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -1999,17 +2039,17 @@
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -2036,12 +2076,12 @@
       <c r="H43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I43" s="18" t="s">
+      <c r="I43" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -2062,15 +2102,15 @@
       <c r="G44" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H44" s="22" t="s">
+      <c r="H44" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I44" s="22" t="s">
+      <c r="I44" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+      <c r="A45" s="17"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -2081,7 +2121,7 @@
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -2092,7 +2132,7 @@
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2103,7 +2143,7 @@
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="21"/>
+      <c r="A48" s="18"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
@@ -2148,32 +2188,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="17"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2200,7 +2240,7 @@
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="3" t="s">
@@ -2208,7 +2248,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2229,10 +2269,10 @@
       <c r="G4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="7" t="s">
@@ -2240,7 +2280,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -2252,7 +2292,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -2264,7 +2304,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -2276,7 +2316,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -2289,18 +2329,18 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="17"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -2327,7 +2367,7 @@
       <c r="H11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J11" s="3" t="s">
@@ -2335,7 +2375,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -2356,10 +2396,10 @@
       <c r="G12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J12" s="7" t="s">
@@ -2367,7 +2407,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -2379,7 +2419,7 @@
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -2391,7 +2431,7 @@
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -2403,7 +2443,7 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -2416,18 +2456,18 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="17"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -2454,7 +2494,7 @@
       <c r="H19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="I19" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J19" s="3" t="s">
@@ -2462,7 +2502,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -2483,10 +2523,10 @@
       <c r="G20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="I20" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J20" s="7" t="s">
@@ -2494,7 +2534,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -2506,7 +2546,7 @@
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -2518,7 +2558,7 @@
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -2530,7 +2570,7 @@
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -2543,18 +2583,18 @@
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="17"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="14"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -2581,7 +2621,7 @@
       <c r="H27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I27" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J27" s="3" t="s">
@@ -2589,7 +2629,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -2610,10 +2650,10 @@
       <c r="G28" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J28" s="7" t="s">
@@ -2621,7 +2661,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -2633,7 +2673,7 @@
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -2645,7 +2685,7 @@
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -2657,7 +2697,7 @@
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -2670,18 +2710,18 @@
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="17"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="14"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -2708,7 +2748,7 @@
       <c r="H35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I35" s="18" t="s">
+      <c r="I35" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J35" s="3" t="s">
@@ -2716,7 +2756,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -2737,10 +2777,10 @@
       <c r="G36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H36" s="22" t="s">
+      <c r="H36" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I36" s="22" t="s">
+      <c r="I36" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J36" s="7" t="s">
@@ -2748,7 +2788,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -2760,7 +2800,7 @@
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
+      <c r="A38" s="17"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -2772,7 +2812,7 @@
       <c r="J38" s="7"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
+      <c r="A39" s="17"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -2784,7 +2824,7 @@
       <c r="J39" s="7"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
@@ -2797,12 +2837,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A34:I34"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A18:I18"/>
     <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A34:I34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2831,32 +2871,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="17"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2883,7 +2923,7 @@
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="15" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="3" t="s">
@@ -2891,7 +2931,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2910,10 +2950,10 @@
       <c r="G4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="19" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="7" t="s">
@@ -2921,7 +2961,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -2933,7 +2973,7 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -2945,7 +2985,7 @@
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -2957,7 +2997,7 @@
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -2980,10 +3020,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2998,32 +3038,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -3041,7 +3081,7 @@
       <c r="E3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="37" t="s">
         <v>45</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -3058,7 +3098,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3067,14 +3107,14 @@
       <c r="C4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="20">
         <v>44393</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="20">
         <v>44407</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>35</v>
+      <c r="F4" s="38" t="s">
+        <v>96</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>46</v>
@@ -3085,57 +3125,85 @@
       <c r="I4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="19" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E10" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3163,22 +3231,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -3198,7 +3266,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -3207,36 +3275,36 @@
       <c r="C4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="21">
         <v>13.8314719</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="22">
         <v>100.53903800000001</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>

</xml_diff>